<commit_message>
final commit with improved swaptions pricing
</commit_message>
<xml_diff>
--- a/opt_data/sample_Simulated_Swaption_Price_imputed.xlsx
+++ b/opt_data/sample_Simulated_Swaption_Price_imputed.xlsx
@@ -5695,7 +5695,9 @@
       <c r="K8" t="n">
         <v>0.035153459998358</v>
       </c>
-      <c r="L8" t="inlineStr"/>
+      <c r="L8" t="n">
+        <v>0.03512404007820401</v>
+      </c>
       <c r="M8" t="n">
         <v>0.0335652178003043</v>
       </c>
@@ -6323,7 +6325,7 @@
         <v>0.0394531566910714</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.0310972850948506</v>
+        <v>0.04203954205791236</v>
       </c>
       <c r="D9" t="n">
         <v>0.0416416766395895</v>
@@ -6985,45 +6987,65 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.1454445781694752</v>
+        <v>0.02981055223042308</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.2994797849993104</v>
+        <v>0.03965627658747125</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.08087260147710879</v>
+        <v>0.04163801216386761</v>
       </c>
       <c r="D10" t="n">
-        <v>0.05964363414271781</v>
+        <v>0.04214682721648869</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.1210732642949498</v>
+        <v>0.04175318980681017</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.05901502716222286</v>
+        <v>0.04045105685498676</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.07510230149383545</v>
+        <v>0.03909522527921545</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.06836337267181546</v>
+        <v>0.03865774304801105</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.06161656039415006</v>
+        <v>0.03818794853771629</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.07267984484381801</v>
-      </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
+        <v>0.0371882216317551</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.03577007278476298</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.03530461514376117</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.03408331784854801</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.03461888564544432</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.05948296948722619</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.07193080535559436</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.07290062380123619</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.07228968475931551</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.07254554499864518</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.06874895844817834</v>
+      </c>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
@@ -7239,45 +7261,65 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.1526391493401427</v>
+        <v>0.02932228549105412</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.06697393852876321</v>
+        <v>0.03984764296168757</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.1055145106251853</v>
+        <v>0.04186578508891921</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.08907363701002781</v>
+        <v>0.04189569415510519</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.136235992353375</v>
+        <v>0.04157940804560083</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.05646531257073401</v>
+        <v>0.04033649575817468</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.06342263177972532</v>
+        <v>0.038873063466944</v>
       </c>
       <c r="H11" t="n">
-        <v>0.01642257192556831</v>
+        <v>0.03848278365276686</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.005184265639627816</v>
+        <v>0.03828519165925346</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.02232177002535096</v>
-      </c>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
+        <v>0.03727591843567041</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.03567816130210945</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.03556955736915279</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.03388301946643414</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.03458231858363352</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.05923304362540343</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.07087891697282364</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.07258383751452631</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.07191402695244994</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.07175975062622075</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.06850281333107071</v>
+      </c>
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
@@ -7493,45 +7535,65 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-0.1006711321764894</v>
+        <v>0.02992784945695767</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.246987492218272</v>
+        <v>0.03950021223192253</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.02675658667644532</v>
+        <v>0.04223306736861817</v>
       </c>
       <c r="D12" t="n">
-        <v>0.01012154391607409</v>
+        <v>0.04198572691094003</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.02998110286543734</v>
+        <v>0.04172338993320767</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.1028156452631753</v>
+        <v>0.04061577231239526</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.0424126182483002</v>
+        <v>0.03916751140102503</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.09204681286092864</v>
+        <v>0.03902982157001228</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.1938739093772585</v>
+        <v>0.03859057569916555</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.1481352916538124</v>
-      </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
-      <c r="T12" t="inlineStr"/>
+        <v>0.03733385581717758</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.03577160914090414</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.03567528164044301</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.03423204542047387</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.034700272720206</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.05973685582122366</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.07227757165249807</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.07287464463656372</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.07207709317290208</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.0717755078077453</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.06872032540536609</v>
+      </c>
       <c r="U12" t="inlineStr"/>
       <c r="V12" t="inlineStr"/>
       <c r="W12" t="inlineStr"/>

</xml_diff>